<commit_message>
Added test workbook for xls
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/named-ranges.xlsx
+++ b/tests/testthat/sheets/named-ranges.xlsx
@@ -8,18 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Albert\Coding\readxl\tests\testthat\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEF39D3A-DD0C-4614-834D-A4F444C8CD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FC78FA-F81C-41B9-AFED-17E9A0BFB622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{8ED11F18-0AC2-4E35-AAFC-26D12192AD32}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="1" xr2:uid="{8ED11F18-0AC2-4E35-AAFC-26D12192AD32}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="apple" localSheetId="0">Sheet1!$I$11:$L$14</definedName>
+    <definedName name="apple" localSheetId="1">Sheet1!$I$11:$L$14</definedName>
     <definedName name="apple">Sheet1!$D$5:$F$11</definedName>
     <definedName name="banana">Sheet1!$F$18:$H$22</definedName>
-    <definedName name="pear" localSheetId="0">Sheet1!$M$3</definedName>
+    <definedName name="blueberry" localSheetId="0">Sheet2!$D$3:$G$3</definedName>
+    <definedName name="peach">'[1]head(mtcars)'!$A$1:$K$7</definedName>
+    <definedName name="pear" localSheetId="1">Sheet1!$M$3</definedName>
+    <definedName name="pineapple">PI()</definedName>
+    <definedName name="raspberry">Sheet2!$B$3:$B$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,6 +49,35 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>BBB</t>
+  </si>
+  <si>
+    <t>CCC</t>
+  </si>
+  <si>
+    <t>DDD</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -52,7 +89,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,6 +120,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -96,12 +145,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -117,6 +168,268 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="head(mtcars)"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>mpg</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>cyl</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>disp</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>hp</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>drat</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>wt</v>
+          </cell>
+          <cell r="G1" t="str">
+            <v>qsec</v>
+          </cell>
+          <cell r="H1" t="str">
+            <v>vs</v>
+          </cell>
+          <cell r="I1" t="str">
+            <v>am</v>
+          </cell>
+          <cell r="J1" t="str">
+            <v>gear</v>
+          </cell>
+          <cell r="K1" t="str">
+            <v>carb</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>21</v>
+          </cell>
+          <cell r="B2">
+            <v>6</v>
+          </cell>
+          <cell r="C2">
+            <v>160</v>
+          </cell>
+          <cell r="D2">
+            <v>110</v>
+          </cell>
+          <cell r="E2">
+            <v>3.9</v>
+          </cell>
+          <cell r="F2">
+            <v>2.62</v>
+          </cell>
+          <cell r="G2">
+            <v>16.46</v>
+          </cell>
+          <cell r="H2">
+            <v>0</v>
+          </cell>
+          <cell r="I2">
+            <v>1</v>
+          </cell>
+          <cell r="J2">
+            <v>4</v>
+          </cell>
+          <cell r="K2">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>21</v>
+          </cell>
+          <cell r="B3">
+            <v>6</v>
+          </cell>
+          <cell r="C3">
+            <v>160</v>
+          </cell>
+          <cell r="D3">
+            <v>110</v>
+          </cell>
+          <cell r="E3">
+            <v>3.9</v>
+          </cell>
+          <cell r="F3">
+            <v>2.875</v>
+          </cell>
+          <cell r="G3">
+            <v>17.02</v>
+          </cell>
+          <cell r="H3">
+            <v>0</v>
+          </cell>
+          <cell r="I3">
+            <v>1</v>
+          </cell>
+          <cell r="J3">
+            <v>4</v>
+          </cell>
+          <cell r="K3">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>22.8</v>
+          </cell>
+          <cell r="B4">
+            <v>4</v>
+          </cell>
+          <cell r="C4">
+            <v>108</v>
+          </cell>
+          <cell r="D4">
+            <v>93</v>
+          </cell>
+          <cell r="E4">
+            <v>3.85</v>
+          </cell>
+          <cell r="F4">
+            <v>2.3199999999999998</v>
+          </cell>
+          <cell r="G4">
+            <v>18.61</v>
+          </cell>
+          <cell r="H4">
+            <v>1</v>
+          </cell>
+          <cell r="I4">
+            <v>1</v>
+          </cell>
+          <cell r="J4">
+            <v>4</v>
+          </cell>
+          <cell r="K4">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>21.4</v>
+          </cell>
+          <cell r="B5">
+            <v>6</v>
+          </cell>
+          <cell r="C5">
+            <v>258</v>
+          </cell>
+          <cell r="D5">
+            <v>110</v>
+          </cell>
+          <cell r="E5">
+            <v>3.08</v>
+          </cell>
+          <cell r="F5">
+            <v>3.2149999999999999</v>
+          </cell>
+          <cell r="G5">
+            <v>19.440000000000001</v>
+          </cell>
+          <cell r="H5">
+            <v>1</v>
+          </cell>
+          <cell r="I5">
+            <v>0</v>
+          </cell>
+          <cell r="J5">
+            <v>3</v>
+          </cell>
+          <cell r="K5">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>18.7</v>
+          </cell>
+          <cell r="B6">
+            <v>8</v>
+          </cell>
+          <cell r="C6">
+            <v>360</v>
+          </cell>
+          <cell r="D6">
+            <v>175</v>
+          </cell>
+          <cell r="E6">
+            <v>3.15</v>
+          </cell>
+          <cell r="F6">
+            <v>3.44</v>
+          </cell>
+          <cell r="G6">
+            <v>17.02</v>
+          </cell>
+          <cell r="H6">
+            <v>0</v>
+          </cell>
+          <cell r="I6">
+            <v>0</v>
+          </cell>
+          <cell r="J6">
+            <v>3</v>
+          </cell>
+          <cell r="K6">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>18.100000000000001</v>
+          </cell>
+          <cell r="B7">
+            <v>6</v>
+          </cell>
+          <cell r="C7">
+            <v>225</v>
+          </cell>
+          <cell r="D7">
+            <v>105</v>
+          </cell>
+          <cell r="E7">
+            <v>2.76</v>
+          </cell>
+          <cell r="F7">
+            <v>3.46</v>
+          </cell>
+          <cell r="G7">
+            <v>20.22</v>
+          </cell>
+          <cell r="H7">
+            <v>1</v>
+          </cell>
+          <cell r="I7">
+            <v>0</v>
+          </cell>
+          <cell r="J7">
+            <v>3</v>
+          </cell>
+          <cell r="K7">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -415,12 +728,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0689486-445A-4F42-A71D-54D85626A09A}">
+  <dimension ref="B3:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93780CC4-A5CF-4BE5-91AA-59D6BC2BB481}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
updated xlsx test file to match xls
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/named-ranges.xlsx
+++ b/tests/testthat/sheets/named-ranges.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,32 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Albert\Coding\readxl\tests\testthat\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FC78FA-F81C-41B9-AFED-17E9A0BFB622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C86F7B7-2BC3-45D7-8FEC-434FFD24F30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="1" xr2:uid="{8ED11F18-0AC2-4E35-AAFC-26D12192AD32}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet 2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="apple" localSheetId="1">Sheet1!$I$11:$L$14</definedName>
     <definedName name="apple">Sheet1!$D$5:$F$11</definedName>
     <definedName name="banana">Sheet1!$F$18:$H$22</definedName>
-    <definedName name="blueberry" localSheetId="0">Sheet2!$D$3:$G$3</definedName>
+    <definedName name="blueberry" localSheetId="0">'Sheet 2'!$D$3:$G$3</definedName>
+    <definedName name="fruit">'Sheet 2'!$1:$1048576</definedName>
+    <definedName name="grapefruit">'Sheet 2:Sheet3'!$D$3</definedName>
+    <definedName name="grapes">Sheet1!$31:$31</definedName>
+    <definedName name="guava">'Sheet 2:Sheet1'!$B$3:$B$5</definedName>
+    <definedName name="lemon" localSheetId="0">Sheet1!$B$19:$C$24</definedName>
+    <definedName name="orange" localSheetId="0">'Sheet 2'!$D$8</definedName>
+    <definedName name="orange">Sheet1!$O:$O</definedName>
+    <definedName name="passionfruit">Sheet1!$R:$T</definedName>
     <definedName name="peach">'[1]head(mtcars)'!$A$1:$K$7</definedName>
     <definedName name="pear" localSheetId="1">Sheet1!$M$3</definedName>
     <definedName name="pineapple">PI()</definedName>
-    <definedName name="raspberry">Sheet2!$B$3:$B$6</definedName>
+    <definedName name="raspberry">'Sheet 2'!$B$3:$B$6</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -50,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>North</t>
   </si>
@@ -75,11 +81,14 @@
   <si>
     <t>DDD</t>
   </si>
+  <si>
+    <t>New York</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,7 +98,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,6 +141,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -145,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -153,6 +186,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -173,9 +210,6 @@
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="head(mtcars)"/>
     </sheetNames>
@@ -728,10 +762,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0689486-445A-4F42-A71D-54D85626A09A}">
-  <dimension ref="B3:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -767,18 +803,29 @@
         <v>3</v>
       </c>
     </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D8" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93780CC4-A5CF-4BE5-91AA-59D6BC2BB481}">
-  <dimension ref="A1:O27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O65536"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="9" style="7"/>
+    <col min="18" max="20" width="9" style="10"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -823,7 +870,7 @@
       <c r="N1">
         <v>38</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="7">
         <v>55</v>
       </c>
     </row>
@@ -870,7 +917,7 @@
       <c r="N2">
         <v>66</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="7">
         <v>76</v>
       </c>
     </row>
@@ -917,7 +964,7 @@
       <c r="N3">
         <v>56</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="7">
         <v>95</v>
       </c>
     </row>
@@ -964,7 +1011,7 @@
       <c r="N4">
         <v>44</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="7">
         <v>28</v>
       </c>
     </row>
@@ -1011,7 +1058,7 @@
       <c r="N5">
         <v>36</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="7">
         <v>80</v>
       </c>
     </row>
@@ -1058,7 +1105,7 @@
       <c r="N6">
         <v>46</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="7">
         <v>61</v>
       </c>
     </row>
@@ -1105,7 +1152,7 @@
       <c r="N7">
         <v>34</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="7">
         <v>46</v>
       </c>
     </row>
@@ -1152,7 +1199,7 @@
       <c r="N8">
         <v>36</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="7">
         <v>6</v>
       </c>
     </row>
@@ -1199,7 +1246,7 @@
       <c r="N9">
         <v>20</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="7">
         <v>78</v>
       </c>
     </row>
@@ -1246,7 +1293,7 @@
       <c r="N10">
         <v>25</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="7">
         <v>81</v>
       </c>
     </row>
@@ -1293,7 +1340,7 @@
       <c r="N11">
         <v>70</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="7">
         <v>40</v>
       </c>
     </row>
@@ -1340,7 +1387,7 @@
       <c r="N12">
         <v>61</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="7">
         <v>39</v>
       </c>
     </row>
@@ -1387,7 +1434,7 @@
       <c r="N13">
         <v>14</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="7">
         <v>55</v>
       </c>
     </row>
@@ -1434,7 +1481,7 @@
       <c r="N14">
         <v>80</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="7">
         <v>68</v>
       </c>
     </row>
@@ -1481,7 +1528,7 @@
       <c r="N15">
         <v>16</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="7">
         <v>89</v>
       </c>
     </row>
@@ -1528,11 +1575,11 @@
       <c r="N16">
         <v>86</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="7">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>18</v>
       </c>
@@ -1575,11 +1622,11 @@
       <c r="N17">
         <v>33</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>31</v>
       </c>
@@ -1622,18 +1669,18 @@
       <c r="N18">
         <v>70</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>23</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="8">
         <v>38</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="8">
         <v>28</v>
       </c>
       <c r="D19">
@@ -1669,18 +1716,18 @@
       <c r="N19">
         <v>46</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="7">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="8">
         <v>7</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="8">
         <v>51</v>
       </c>
       <c r="D20">
@@ -1716,18 +1763,18 @@
       <c r="N20">
         <v>29</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="7">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>48</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="8">
         <v>8</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="8">
         <v>28</v>
       </c>
       <c r="D21">
@@ -1763,18 +1810,18 @@
       <c r="N21">
         <v>26</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="7">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>60</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="8">
         <v>50</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="8">
         <v>6</v>
       </c>
       <c r="D22">
@@ -1810,18 +1857,18 @@
       <c r="N22">
         <v>35</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="7">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="8">
         <v>22</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="8">
         <v>60</v>
       </c>
       <c r="D23">
@@ -1857,18 +1904,18 @@
       <c r="N23">
         <v>57</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="7">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>13</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="8">
         <v>41</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="8">
         <v>10</v>
       </c>
       <c r="D24">
@@ -1904,11 +1951,11 @@
       <c r="N24">
         <v>5</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="7">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>69</v>
       </c>
@@ -1951,11 +1998,11 @@
       <c r="N25">
         <v>36</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="7">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>37</v>
       </c>
@@ -1998,11 +2045,11 @@
       <c r="N26">
         <v>30</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="7">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>82</v>
       </c>
@@ -2045,11 +2092,123 @@
       <c r="N27">
         <v>63</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="7">
         <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>1</v>
+      </c>
+      <c r="B31" s="9">
+        <v>1</v>
+      </c>
+      <c r="C31" s="9">
+        <f>A31+B31</f>
+        <v>2</v>
+      </c>
+      <c r="D31" s="9">
+        <f t="shared" ref="D31:Y31" si="0">B31+C31</f>
+        <v>3</v>
+      </c>
+      <c r="E31" s="9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F31" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G31" s="9">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="H31" s="9">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="I31" s="9">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="J31" s="9">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="K31" s="9">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="L31" s="9">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="M31" s="9">
+        <f t="shared" si="0"/>
+        <v>233</v>
+      </c>
+      <c r="N31" s="9">
+        <f t="shared" si="0"/>
+        <v>377</v>
+      </c>
+      <c r="O31" s="9">
+        <f t="shared" si="0"/>
+        <v>610</v>
+      </c>
+      <c r="P31" s="9">
+        <f t="shared" si="0"/>
+        <v>987</v>
+      </c>
+      <c r="Q31" s="9">
+        <f t="shared" si="0"/>
+        <v>1597</v>
+      </c>
+      <c r="R31" s="10">
+        <f t="shared" si="0"/>
+        <v>2584</v>
+      </c>
+      <c r="S31" s="10">
+        <f t="shared" si="0"/>
+        <v>4181</v>
+      </c>
+      <c r="T31" s="10">
+        <f t="shared" si="0"/>
+        <v>6765</v>
+      </c>
+      <c r="U31" s="9">
+        <f t="shared" si="0"/>
+        <v>10946</v>
+      </c>
+      <c r="V31" s="9">
+        <f t="shared" si="0"/>
+        <v>17711</v>
+      </c>
+      <c r="W31" s="9">
+        <f t="shared" si="0"/>
+        <v>28657</v>
+      </c>
+      <c r="X31" s="9">
+        <f t="shared" si="0"/>
+        <v>46368</v>
+      </c>
+      <c r="Y31" s="9">
+        <f t="shared" si="0"/>
+        <v>75025</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>